<commit_message>
added warning message and renamed the excel sheet
</commit_message>
<xml_diff>
--- a/templates/Excel/ST1/ST1_Line_Rejection.xlsx
+++ b/templates/Excel/ST1/ST1_Line_Rejection.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2332,74 +2332,1484 @@
           <t>SHIFT1</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>645</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
+      <c r="C33" t="n">
+        <v>645</v>
+      </c>
+      <c r="D33" t="n">
+        <v>654</v>
+      </c>
+      <c r="E33" t="n">
+        <v>64</v>
+      </c>
+      <c r="F33" t="n">
+        <v>64</v>
+      </c>
+      <c r="G33" t="n">
+        <v>646</v>
+      </c>
+      <c r="H33" t="n">
+        <v>46</v>
+      </c>
+      <c r="I33" t="n">
+        <v>46</v>
+      </c>
+      <c r="J33" t="n">
+        <v>46</v>
+      </c>
+      <c r="K33" t="n">
+        <v>46</v>
+      </c>
+      <c r="L33" t="n">
+        <v>46</v>
+      </c>
+      <c r="M33" t="n">
+        <v>4</v>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>646</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-01-31T16:44</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D34" t="n">
+        <v>456</v>
+      </c>
+      <c r="E34" t="n">
+        <v>564</v>
+      </c>
+      <c r="F34" t="n">
+        <v>64</v>
+      </c>
+      <c r="G34" t="n">
+        <v>64</v>
+      </c>
+      <c r="H34" t="n">
+        <v>646</v>
+      </c>
+      <c r="I34" t="n">
+        <v>6</v>
+      </c>
+      <c r="J34" t="n">
+        <v>46</v>
+      </c>
+      <c r="K34" t="n">
+        <v>46</v>
+      </c>
+      <c r="L34" t="n">
+        <v>46</v>
+      </c>
+      <c r="M34" t="n">
+        <v>464</v>
+      </c>
+      <c r="N34" t="inlineStr">
         <is>
           <t>654</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="O34" t="inlineStr">
         <is>
           <t>64</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="P34" t="inlineStr">
         <is>
           <t>64</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-02-11T16:57</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>52</v>
+      </c>
+      <c r="D35" t="n">
+        <v>65</v>
+      </c>
+      <c r="E35" t="n">
+        <v>564</v>
+      </c>
+      <c r="F35" t="n">
+        <v>654</v>
+      </c>
+      <c r="G35" t="n">
+        <v>64</v>
+      </c>
+      <c r="H35" t="n">
+        <v>64</v>
+      </c>
+      <c r="I35" t="n">
+        <v>6</v>
+      </c>
+      <c r="J35" t="n">
+        <v>4</v>
+      </c>
+      <c r="K35" t="n">
+        <v>64</v>
+      </c>
+      <c r="L35" t="n">
+        <v>64</v>
+      </c>
+      <c r="M35" t="n">
+        <v>64</v>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
         <is>
           <t>646</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-02-11T16:57</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>52</v>
+      </c>
+      <c r="D36" t="n">
+        <v>65</v>
+      </c>
+      <c r="E36" t="n">
+        <v>564</v>
+      </c>
+      <c r="F36" t="n">
+        <v>654</v>
+      </c>
+      <c r="G36" t="n">
+        <v>64</v>
+      </c>
+      <c r="H36" t="n">
+        <v>64</v>
+      </c>
+      <c r="I36" t="n">
+        <v>6</v>
+      </c>
+      <c r="J36" t="n">
+        <v>4</v>
+      </c>
+      <c r="K36" t="n">
+        <v>64</v>
+      </c>
+      <c r="L36" t="n">
+        <v>64</v>
+      </c>
+      <c r="M36" t="n">
+        <v>64</v>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>646</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-02-06T17:01</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>645</v>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="n">
+        <v>654</v>
+      </c>
+      <c r="F37" t="n">
+        <v>64</v>
+      </c>
+      <c r="G37" t="n">
+        <v>64</v>
+      </c>
+      <c r="H37" t="n">
+        <v>64</v>
+      </c>
+      <c r="I37" t="n">
+        <v>646</v>
+      </c>
+      <c r="J37" t="n">
+        <v>46</v>
+      </c>
+      <c r="K37" t="n">
+        <v>6</v>
+      </c>
+      <c r="L37" t="n">
+        <v>46</v>
+      </c>
+      <c r="M37" t="n">
+        <v>46</v>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-02-05T17:03</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>234</v>
+      </c>
+      <c r="D38" t="n">
+        <v>654</v>
+      </c>
+      <c r="E38" t="n">
+        <v>654</v>
+      </c>
+      <c r="F38" t="n">
+        <v>646</v>
+      </c>
+      <c r="G38" t="n">
+        <v>464</v>
+      </c>
+      <c r="H38" t="n">
+        <v>64</v>
+      </c>
+      <c r="I38" t="n">
+        <v>6</v>
+      </c>
+      <c r="J38" t="n">
+        <v>6</v>
+      </c>
+      <c r="K38" t="n">
+        <v>6</v>
+      </c>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="n">
+        <v>6</v>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-02-05T17:03</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>234</v>
+      </c>
+      <c r="D39" t="n">
+        <v>654</v>
+      </c>
+      <c r="E39" t="n">
+        <v>654</v>
+      </c>
+      <c r="F39" t="n">
+        <v>646</v>
+      </c>
+      <c r="G39" t="n">
+        <v>464</v>
+      </c>
+      <c r="H39" t="n">
+        <v>64</v>
+      </c>
+      <c r="I39" t="n">
+        <v>6</v>
+      </c>
+      <c r="J39" t="n">
+        <v>6</v>
+      </c>
+      <c r="K39" t="n">
+        <v>6</v>
+      </c>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="n">
+        <v>6</v>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-02-14T17:04</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>54648</v>
+      </c>
+      <c r="D40" t="n">
+        <v>64</v>
+      </c>
+      <c r="E40" t="n">
+        <v>64</v>
+      </c>
+      <c r="F40" t="n">
+        <v>64</v>
+      </c>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="n">
+        <v>6</v>
+      </c>
+      <c r="I40" t="n">
+        <v>4</v>
+      </c>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="n">
+        <v>4</v>
+      </c>
+      <c r="L40" t="n">
+        <v>4</v>
+      </c>
+      <c r="M40" t="n">
+        <v>4</v>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-02-14T17:04</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>54648</v>
+      </c>
+      <c r="D41" t="n">
+        <v>64</v>
+      </c>
+      <c r="E41" t="n">
+        <v>64</v>
+      </c>
+      <c r="F41" t="n">
+        <v>64</v>
+      </c>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="n">
+        <v>6</v>
+      </c>
+      <c r="I41" t="n">
+        <v>4</v>
+      </c>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="n">
+        <v>4</v>
+      </c>
+      <c r="L41" t="n">
+        <v>4</v>
+      </c>
+      <c r="M41" t="n">
+        <v>4</v>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-02-06T17:06</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="n">
+        <v>41</v>
+      </c>
+      <c r="D42" t="n">
+        <v>4</v>
+      </c>
+      <c r="E42" t="n">
+        <v>4</v>
+      </c>
+      <c r="F42" t="n">
+        <v>4</v>
+      </c>
+      <c r="G42" t="n">
+        <v>4</v>
+      </c>
+      <c r="H42" t="n">
+        <v>4</v>
+      </c>
+      <c r="I42" t="n">
+        <v>4</v>
+      </c>
+      <c r="J42" t="n">
+        <v>4</v>
+      </c>
+      <c r="K42" t="n">
+        <v>4</v>
+      </c>
+      <c r="L42" t="n">
+        <v>44</v>
+      </c>
+      <c r="M42" t="n">
+        <v>4</v>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-02-05T17:11</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>864</v>
+      </c>
+      <c r="D43" t="n">
+        <v>8</v>
+      </c>
+      <c r="E43" t="n">
+        <v>8</v>
+      </c>
+      <c r="F43" t="n">
+        <v>8</v>
+      </c>
+      <c r="G43" t="n">
+        <v>8</v>
+      </c>
+      <c r="H43" t="n">
+        <v>8</v>
+      </c>
+      <c r="I43" t="n">
+        <v>8</v>
+      </c>
+      <c r="J43" t="n">
+        <v>8</v>
+      </c>
+      <c r="K43" t="n">
+        <v>8</v>
+      </c>
+      <c r="L43" t="n">
+        <v>8</v>
+      </c>
+      <c r="M43" t="n">
+        <v>8</v>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-02-05T17:12</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>465</v>
+      </c>
+      <c r="D44" t="n">
+        <v>8</v>
+      </c>
+      <c r="E44" t="n">
+        <v>8</v>
+      </c>
+      <c r="F44" t="n">
+        <v>8</v>
+      </c>
+      <c r="G44" t="n">
+        <v>8</v>
+      </c>
+      <c r="H44" t="n">
+        <v>88</v>
+      </c>
+      <c r="I44" t="n">
+        <v>8</v>
+      </c>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="n">
+        <v>8</v>
+      </c>
+      <c r="L44" t="n">
+        <v>8</v>
+      </c>
+      <c r="M44" t="n">
+        <v>8</v>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-02-05T17:14</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-02-05T17:14</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-02-04T17:16</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>456</v>
+      </c>
+      <c r="D47" t="n">
+        <v>45</v>
+      </c>
+      <c r="E47" t="n">
+        <v>45</v>
+      </c>
+      <c r="F47" t="n">
+        <v>45</v>
+      </c>
+      <c r="G47" t="n">
+        <v>4545</v>
+      </c>
+      <c r="H47" t="n">
+        <v>45</v>
+      </c>
+      <c r="I47" t="n">
+        <v>45</v>
+      </c>
+      <c r="J47" t="n">
+        <v>4545</v>
+      </c>
+      <c r="K47" t="n">
+        <v>45</v>
+      </c>
+      <c r="L47" t="n">
+        <v>45</v>
+      </c>
+      <c r="M47" t="n">
+        <v>45</v>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-02-04T17:16</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>456</v>
+      </c>
+      <c r="D48" t="n">
+        <v>45</v>
+      </c>
+      <c r="E48" t="n">
+        <v>45</v>
+      </c>
+      <c r="F48" t="n">
+        <v>45</v>
+      </c>
+      <c r="G48" t="n">
+        <v>4545</v>
+      </c>
+      <c r="H48" t="n">
+        <v>45</v>
+      </c>
+      <c r="I48" t="n">
+        <v>45</v>
+      </c>
+      <c r="J48" t="n">
+        <v>4545</v>
+      </c>
+      <c r="K48" t="n">
+        <v>45</v>
+      </c>
+      <c r="L48" t="n">
+        <v>45</v>
+      </c>
+      <c r="M48" t="n">
+        <v>45</v>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-01-29T17:17</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>4</v>
+      </c>
+      <c r="D49" t="n">
+        <v>7</v>
+      </c>
+      <c r="E49" t="n">
+        <v>7</v>
+      </c>
+      <c r="F49" t="n">
+        <v>7</v>
+      </c>
+      <c r="G49" t="n">
+        <v>7</v>
+      </c>
+      <c r="H49" t="n">
+        <v>7</v>
+      </c>
+      <c r="I49" t="n">
+        <v>7</v>
+      </c>
+      <c r="J49" t="n">
+        <v>7</v>
+      </c>
+      <c r="K49" t="n">
+        <v>7</v>
+      </c>
+      <c r="L49" t="n">
+        <v>7</v>
+      </c>
+      <c r="M49" t="n">
+        <v>7</v>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-02-12T17:21</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>56</v>
+      </c>
+      <c r="D51" t="n">
+        <v>56</v>
+      </c>
+      <c r="E51" t="n">
+        <v>56</v>
+      </c>
+      <c r="F51" t="n">
+        <v>5656</v>
+      </c>
+      <c r="G51" t="n">
+        <v>65</v>
+      </c>
+      <c r="H51" t="n">
+        <v>65</v>
+      </c>
+      <c r="I51" t="n">
+        <v>54</v>
+      </c>
+      <c r="J51" t="n">
+        <v>45</v>
+      </c>
+      <c r="K51" t="n">
+        <v>4</v>
+      </c>
+      <c r="L51" t="n">
+        <v>4</v>
+      </c>
+      <c r="M51" t="n">
+        <v>65</v>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-02-12T17:21</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>56</v>
+      </c>
+      <c r="D52" t="n">
+        <v>56</v>
+      </c>
+      <c r="E52" t="n">
+        <v>56</v>
+      </c>
+      <c r="F52" t="n">
+        <v>5656</v>
+      </c>
+      <c r="G52" t="n">
+        <v>65</v>
+      </c>
+      <c r="H52" t="n">
+        <v>65</v>
+      </c>
+      <c r="I52" t="n">
+        <v>54</v>
+      </c>
+      <c r="J52" t="n">
+        <v>45</v>
+      </c>
+      <c r="K52" t="n">
+        <v>4</v>
+      </c>
+      <c r="L52" t="n">
+        <v>4</v>
+      </c>
+      <c r="M52" t="n">
+        <v>65</v>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-02-05T17:23</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>4</v>
+      </c>
+      <c r="D53" t="n">
+        <v>5454</v>
+      </c>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="n">
+        <v>5</v>
+      </c>
+      <c r="G53" t="n">
+        <v>5</v>
+      </c>
+      <c r="H53" t="n">
+        <v>54</v>
+      </c>
+      <c r="I53" t="n">
+        <v>45</v>
+      </c>
+      <c r="J53" t="n">
+        <v>45</v>
+      </c>
+      <c r="K53" t="n">
+        <v>4545</v>
+      </c>
+      <c r="L53" t="n">
+        <v>45</v>
+      </c>
+      <c r="M53" t="n">
+        <v>45</v>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-02-05T17:23</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>4</v>
+      </c>
+      <c r="D54" t="n">
+        <v>5454</v>
+      </c>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="n">
+        <v>5</v>
+      </c>
+      <c r="G54" t="n">
+        <v>5</v>
+      </c>
+      <c r="H54" t="n">
+        <v>54</v>
+      </c>
+      <c r="I54" t="n">
+        <v>45</v>
+      </c>
+      <c r="J54" t="n">
+        <v>45</v>
+      </c>
+      <c r="K54" t="n">
+        <v>4545</v>
+      </c>
+      <c r="L54" t="n">
+        <v>45</v>
+      </c>
+      <c r="M54" t="n">
+        <v>45</v>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-02-01T17:26</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>45</v>
+      </c>
+      <c r="D55" t="n">
+        <v>45</v>
+      </c>
+      <c r="E55" t="n">
+        <v>54</v>
+      </c>
+      <c r="F55" t="n">
+        <v>546</v>
+      </c>
+      <c r="G55" t="n">
+        <v>45</v>
+      </c>
+      <c r="H55" t="n">
+        <v>54564</v>
+      </c>
+      <c r="I55" t="n">
+        <v>65</v>
+      </c>
+      <c r="J55" t="n">
+        <v>6</v>
+      </c>
+      <c r="K55" t="n">
+        <v>6</v>
+      </c>
+      <c r="L55" t="n">
+        <v>6</v>
+      </c>
+      <c r="M55" t="n">
+        <v>6</v>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-01-29T17:26</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>4</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1</v>
+      </c>
+      <c r="F56" t="n">
+        <v>1</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1</v>
+      </c>
+      <c r="H56" t="n">
+        <v>1</v>
+      </c>
+      <c r="I56" t="n">
+        <v>1</v>
+      </c>
+      <c r="J56" t="n">
+        <v>1</v>
+      </c>
+      <c r="K56" t="n">
+        <v>1</v>
+      </c>
+      <c r="L56" t="n">
+        <v>1</v>
+      </c>
+      <c r="M56" t="n">
+        <v>1</v>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-02-13T17:27</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>546</v>
+      </c>
+      <c r="D57" t="n">
+        <v>564</v>
+      </c>
+      <c r="E57" t="n">
+        <v>456</v>
+      </c>
+      <c r="F57" t="n">
+        <v>645</v>
+      </c>
+      <c r="G57" t="n">
+        <v>645</v>
+      </c>
+      <c r="H57" t="n">
+        <v>64</v>
+      </c>
+      <c r="I57" t="n">
+        <v>646</v>
+      </c>
+      <c r="J57" t="n">
+        <v>464</v>
+      </c>
+      <c r="K57" t="n">
+        <v>64</v>
+      </c>
+      <c r="L57" t="n">
+        <v>6</v>
+      </c>
+      <c r="M57" t="n">
+        <v>46</v>
+      </c>
+      <c r="N57" t="inlineStr">
         <is>
           <t>46</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr">
+      <c r="O57" t="inlineStr">
         <is>
           <t>46</t>
         </is>
       </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>46</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>46</t>
-        </is>
-      </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>46</t>
-        </is>
-      </c>
-      <c r="M33" t="inlineStr">
+      <c r="P57" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="N33" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
-      </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>646</t>
-        </is>
-      </c>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t>46</t>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-01-29T18:13</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>